<commit_message>
load data for march,
</commit_message>
<xml_diff>
--- a/PVL/docs/findErrors.xlsx
+++ b/PVL/docs/findErrors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>File name</t>
   </si>
@@ -42,6 +42,57 @@
   </si>
   <si>
     <t>Column "OneClick"</t>
+  </si>
+  <si>
+    <t>FF_DailyOrder-26032015.csv</t>
+  </si>
+  <si>
+    <t>FF_Account-13032015.csv</t>
+  </si>
+  <si>
+    <t>Row 4, Column 52: String data, right truncation</t>
+  </si>
+  <si>
+    <t>FF_Account-14032015.csv</t>
+  </si>
+  <si>
+    <t>FF_Account-18032015.csv</t>
+  </si>
+  <si>
+    <t>FF_Account-19032015.csv</t>
+  </si>
+  <si>
+    <t>Row 2, Column 52: String data, right truncation</t>
+  </si>
+  <si>
+    <t>Row 15, Column 52: String data, right truncation</t>
+  </si>
+  <si>
+    <t>Row 3, Column 52: String data, right truncation</t>
+  </si>
+  <si>
+    <t>Некорректные данные  в поле ClientUserId</t>
+  </si>
+  <si>
+    <t>Row 16, Column 4: String data, right truncation</t>
+  </si>
+  <si>
+    <t>FF_Order-14032015.csv</t>
+  </si>
+  <si>
+    <t>FF_Order-19032015.csv</t>
+  </si>
+  <si>
+    <t>Row 3, Column 4: String data, right truncation</t>
+  </si>
+  <si>
+    <t>FF_Subscriptions-14032015.csv</t>
+  </si>
+  <si>
+    <t>FF_Subscriptions-19032015.csv</t>
+  </si>
+  <si>
+    <t>Row 1, Column 15: String data, right truncation</t>
   </si>
 </sst>
 </file>
@@ -370,19 +421,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -390,7 +442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -398,12 +450,108 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>